<commit_message>
fix description of C117
</commit_message>
<xml_diff>
--- a/esp32_12chan_lowside_pwm_pcb_v2/pcb_esp32_wled_pwm_multichannel_bom_.xlsx
+++ b/esp32_12chan_lowside_pwm_pcb_v2/pcb_esp32_wled_pwm_multichannel_bom_.xlsx
@@ -178,7 +178,7 @@
     <t xml:space="preserve">C117</t>
   </si>
   <si>
-    <t xml:space="preserve">330µF/16V</t>
+    <t xml:space="preserve">330µF/6.3V</t>
   </si>
   <si>
     <t xml:space="preserve">RVT0J331M0607</t>
@@ -600,6 +600,7 @@
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -702,8 +703,8 @@
   </sheetPr>
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.09765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -711,8 +712,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.85"/>
@@ -995,7 +996,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1005,7 +1006,7 @@
       <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="0" t="s">
         <v>52</v>
       </c>
       <c r="E8" s="1" t="s">

</xml_diff>